<commit_message>
Added questions for quiz
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riyai\OneDrive - Vidyalankar Institute of Technology\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riya\addques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0CF1D99-55C6-4093-B6B4-07EB58E8D743}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF5A0C7-06BB-42DE-9637-F082A721529C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D22A10D-CC82-453F-A65B-3BF5A59E874D}"/>
+    <workbookView xWindow="3972" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{2D1729EE-C6D4-4DFC-8FF3-655793736E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,107 +30,107 @@
     <t>question</t>
   </si>
   <si>
-    <t>choice1</t>
-  </si>
-  <si>
-    <t>choice2</t>
-  </si>
-  <si>
-    <t>choice3</t>
-  </si>
-  <si>
-    <t>choice4</t>
-  </si>
-  <si>
-    <t>answer</t>
+    <t>choice A</t>
+  </si>
+  <si>
+    <t>choice B</t>
+  </si>
+  <si>
+    <t>choice D</t>
+  </si>
+  <si>
+    <t>choice C</t>
+  </si>
+  <si>
+    <t>correct answer</t>
   </si>
   <si>
     <t>domain</t>
   </si>
   <si>
-    <t>Knot is a unit of _________?</t>
-  </si>
-  <si>
-    <t>[A] Speed</t>
-  </si>
-  <si>
-    <t>[B] Distance</t>
-  </si>
-  <si>
-    <t>[C] Deapth</t>
-  </si>
-  <si>
-    <t>[D] Accelration</t>
-  </si>
-  <si>
-    <t>science</t>
-  </si>
-  <si>
-    <t>You are sitting inside an open vehicle moving with uniform speed. When you throw a stone vertically upwards, the stone will fall__:</t>
-  </si>
-  <si>
-    <t>[A] Ahead of you</t>
-  </si>
-  <si>
-    <t>[B] Behind you</t>
-  </si>
-  <si>
-    <t>[C] Over you</t>
-  </si>
-  <si>
-    <t>[D] Either ahead or behind of you</t>
-  </si>
-  <si>
-    <t>Which among the following is the most primitive life form?</t>
-  </si>
-  <si>
-    <t>[A] Bacteria</t>
-  </si>
-  <si>
-    <t>[B] Protozoa</t>
-  </si>
-  <si>
-    <t>[C] Virus</t>
-  </si>
-  <si>
-    <t>[D] Blue-green algae</t>
-  </si>
-  <si>
-    <t>The X-ray crystallography mainly uses which among the following properties of electromagnetic radiation?</t>
-  </si>
-  <si>
-    <t>[A] Reflection</t>
-  </si>
-  <si>
-    <t>[B] Diffraction</t>
-  </si>
-  <si>
-    <t>[C] Interference</t>
-  </si>
-  <si>
-    <t>[D] Refraction</t>
-  </si>
-  <si>
-    <t>An Electric generator is based on which of the following scientific principles?</t>
-  </si>
-  <si>
-    <t>[A] Faraday’s law of Electromagnetic Induction</t>
-  </si>
-  <si>
-    <t>[B] Super Conductivity</t>
-  </si>
-  <si>
-    <t>[C] Laws of Thermodynamics</t>
-  </si>
-  <si>
-    <t>[D] Newton’s Law of Motion</t>
+    <t>agriculture</t>
+  </si>
+  <si>
+    <t>Which of the following is the commercial crop in India?</t>
+  </si>
+  <si>
+    <t>A. Mustard</t>
+  </si>
+  <si>
+    <t>B. tobacco</t>
+  </si>
+  <si>
+    <t>C. Jute</t>
+  </si>
+  <si>
+    <t>D. All of the above</t>
+  </si>
+  <si>
+    <t>Which Indian state produces the largest quantity of pulses?</t>
+  </si>
+  <si>
+    <t>A. Maharashtra</t>
+  </si>
+  <si>
+    <t>B. Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>C. Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>D. Rajasthan</t>
+  </si>
+  <si>
+    <t>What is the correct descending order of rice producing states in India?</t>
+  </si>
+  <si>
+    <t>A. Punjab, West Bengal, Uttar Pradesh And Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>B. Punjab, West Bengal, Uttar Pradesh And Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>C. Punjab, West Bengal, Uttar Pradesh And Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>D. West Bengal, Uttar Pradesh, Punjab, And Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Which of the following is not matched correctly?</t>
+  </si>
+  <si>
+    <t>A. Rabi Crop………Mustard, Cucumber</t>
+  </si>
+  <si>
+    <t>B. Rabi Crop………Mustard, Barley</t>
+  </si>
+  <si>
+    <t>C. Zaid Crop………Moong, vegetables</t>
+  </si>
+  <si>
+    <t>D. Kharif Crop…..Cotton</t>
+  </si>
+  <si>
+    <t>Who approves the Fair and Remunerative Price (FRP) of sugarcane?</t>
+  </si>
+  <si>
+    <t>A. Cabinet Committee on Economic Affairs</t>
+  </si>
+  <si>
+    <t>B. Commission for Agricultural Costs and Prices</t>
+  </si>
+  <si>
+    <t>C. Directorate of Marketing and Inspection, Ministry of Agriculture</t>
+  </si>
+  <si>
+    <t>D. Agricultural Produce Market Committee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,22 +139,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FF2A2A2A"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF090909"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,12 +170,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,160 +490,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED14CB5-DC0E-4E79-8EE0-95701FBDAA3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E68E15-2A7D-42A1-BF0E-A56EC417C9B3}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="113.109375" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="34" customWidth="1"/>
-    <col min="6" max="6" width="41.109375" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="62.33203125" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" customWidth="1"/>
+    <col min="5" max="5" width="45.77734375" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
+      <c r="G3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
+      <c r="G6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>